<commit_message>
Matriz de Trazabilidad de Requerimientos
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/MTREQM/MTREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/MTREQM/MTREQM_V1.1_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\MTREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_REQM\MTREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="151">
   <si>
     <t>HISTORIAL DE LAS REVISIONES</t>
   </si>
@@ -53,18 +53,9 @@
     <t>Responsable de Revisión y/o Aprobación</t>
   </si>
   <si>
-    <t>Version Preliminar</t>
-  </si>
-  <si>
-    <t>En Revisión</t>
-  </si>
-  <si>
     <t>MTREQM Matriz de Trazabilidad de Requerimientos de Documentos</t>
   </si>
   <si>
-    <t>Fecha Efectiva: 13/10/2015</t>
-  </si>
-  <si>
     <t>Objetivo</t>
   </si>
   <si>
@@ -231,9 +222,6 @@
   </si>
   <si>
     <t>DOCUMENTADOR</t>
-  </si>
-  <si>
-    <t>INPRU_V1.0_2015</t>
   </si>
   <si>
     <t>REQ 1.1</t>
@@ -435,12 +423,6 @@
     <t>Roger Apaéstegui</t>
   </si>
   <si>
-    <t>Aprobado</t>
-  </si>
-  <si>
-    <t>Version Preliminar Aprobado por QA</t>
-  </si>
-  <si>
     <t>Julio Leonardo Paredes</t>
   </si>
   <si>
@@ -472,12 +454,39 @@
   </si>
   <si>
     <t>MTREQM MATRIZ DE TRAZABILIDAD DE REQUERIMIENTOS A DOCUMENTOS</t>
+  </si>
+  <si>
+    <t>Version Preliminar Revisada por QA</t>
+  </si>
+  <si>
+    <t>Revisado</t>
+  </si>
+  <si>
+    <t>Version Final pendiente de Aprobación</t>
+  </si>
+  <si>
+    <t>Fecha Efectiva: 19/11/2015</t>
+  </si>
+  <si>
+    <t>MODULO CONFIGURA TU ALARMA</t>
+  </si>
+  <si>
+    <t>MODULO AJUSTES DE LA APLICACIÓN</t>
+  </si>
+  <si>
+    <t>MODULO LISTA DE ALARMAS</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN INTERNA</t>
+  </si>
+  <si>
+    <t>INPRUIN_V1.0_2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1511,18 +1520,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1577,6 +1574,105 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1598,18 +1694,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1618,81 +1702,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1799,6 +1808,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1846,24 +1873,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2445,7 +2454,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2457,99 +2466,99 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="82"/>
-      <c r="B1" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="89"/>
       <c r="I1" s="81"/>
       <c r="J1" s="81"/>
       <c r="K1" s="82"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="82"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="95"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
       <c r="I2" s="82"/>
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="82"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="95"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="82"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
       <c r="I4" s="82"/>
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="95"/>
       <c r="I5" s="82"/>
       <c r="J5" s="82"/>
       <c r="K5" s="82"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="101"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="98"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B7" s="102"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="104"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="B8" s="105"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="107"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="104"/>
     </row>
     <row r="9" spans="1:11" ht="24">
       <c r="B9" s="83" t="s">
@@ -2575,68 +2584,68 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10" s="87">
+      <c r="B10" s="105">
         <v>1</v>
       </c>
-      <c r="C10" s="88" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="89">
+      <c r="C10" s="106" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="107">
         <v>42297</v>
       </c>
-      <c r="E10" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="87" t="s">
-        <v>136</v>
-      </c>
-      <c r="G10" s="87" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="87" t="s">
-        <v>137</v>
+      <c r="E10" s="105" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="105" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="105" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="B12" s="87">
+      <c r="B12" s="105">
         <v>1</v>
       </c>
-      <c r="C12" s="88" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="89">
-        <v>42313</v>
-      </c>
-      <c r="E12" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="87" t="s">
-        <v>137</v>
+      <c r="C12" s="106" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="107">
+        <v>42327</v>
+      </c>
+      <c r="E12" s="105" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="105" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="105" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="B13" s="87"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" s="1"/>
@@ -2649,6 +2658,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="B1:H5"/>
     <mergeCell ref="B6:H8"/>
     <mergeCell ref="B10:B11"/>
@@ -2658,13 +2674,6 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2675,127 +2684,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:12" ht="15" customHeight="1">
-      <c r="B1" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92"/>
+      <c r="B1" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="89"/>
     </row>
     <row r="2" spans="2:12" ht="15" customHeight="1">
-      <c r="B2" s="93"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="95"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="92"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1">
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="95"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="92"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1">
-      <c r="B4" s="93"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="95"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="92"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B5" s="96"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="98"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="95"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B6" s="110" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="115" t="s">
+      <c r="B6" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B7" s="140"/>
+      <c r="C7" s="111" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="113"/>
+    </row>
+    <row r="8" spans="2:12" ht="50.25" customHeight="1" thickBot="1">
+      <c r="B8" s="108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="110"/>
+      <c r="D8" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="138"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="138"/>
-      <c r="J6" s="138"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="116"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B7" s="111"/>
-      <c r="C7" s="139" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140"/>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="141"/>
-    </row>
-    <row r="8" spans="2:12" ht="50.25" customHeight="1" thickBot="1">
-      <c r="B8" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="112" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="113"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
-      <c r="L8" s="114"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
+      <c r="H8" s="142"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="143"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="4"/>
@@ -2811,21 +2820,21 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="142" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="142"/>
+      <c r="B10" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="114"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="143" t="s">
+      <c r="E10" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="144"/>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="144"/>
-      <c r="L10" s="145"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
+      <c r="K10" s="116"/>
+      <c r="L10" s="117"/>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="3"/>
@@ -2841,21 +2850,21 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="146" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="146"/>
+      <c r="B12" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="118"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="135" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="135"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="135"/>
-      <c r="I12" s="135"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="135"/>
+      <c r="E12" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="8"/>
@@ -2871,21 +2880,21 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="134" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="134"/>
+      <c r="B14" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="120"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="135"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
+      <c r="E14" s="119" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="119"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="119"/>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="3"/>
@@ -2901,21 +2910,21 @@
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="121"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="136"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="135" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="135"/>
-      <c r="G16" s="135"/>
-      <c r="H16" s="135"/>
-      <c r="I16" s="135"/>
-      <c r="J16" s="135"/>
-      <c r="K16" s="135"/>
-      <c r="L16" s="135"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="3"/>
@@ -2931,21 +2940,21 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="137"/>
+      <c r="B18" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="122"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="135" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="135"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
-      <c r="L18" s="135"/>
+      <c r="E18" s="119" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="4"/>
@@ -2974,319 +2983,319 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="124" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="124"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="124"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="124"/>
+      <c r="K21" s="124"/>
+      <c r="L21" s="124"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="126"/>
+      <c r="D22" s="127" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="127"/>
+      <c r="K22" s="127"/>
+      <c r="L22" s="127"/>
+    </row>
+    <row r="23" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B23" s="128" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="128"/>
+      <c r="D23" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="126"/>
-      <c r="I21" s="126"/>
-      <c r="J21" s="126"/>
-      <c r="K21" s="126"/>
-      <c r="L21" s="126"/>
-    </row>
-    <row r="22" spans="2:12">
-      <c r="B22" s="127" t="s">
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="130"/>
+      <c r="L23" s="131"/>
+    </row>
+    <row r="24" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B24" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="129" t="s">
+      <c r="C24" s="128"/>
+      <c r="D24" s="132" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
+      <c r="G24" s="132"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="132"/>
+      <c r="J24" s="132"/>
+      <c r="K24" s="132"/>
+      <c r="L24" s="132"/>
+    </row>
+    <row r="25" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B25" s="128" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="128"/>
+      <c r="D25" s="132" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="132"/>
+      <c r="K25" s="132"/>
+      <c r="L25" s="132"/>
+    </row>
+    <row r="26" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B26" s="124" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="124"/>
+    </row>
+    <row r="27" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B27" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="126"/>
+      <c r="D27" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
-      <c r="G22" s="129"/>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="129"/>
-      <c r="K22" s="129"/>
-      <c r="L22" s="129"/>
-    </row>
-    <row r="23" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B23" s="117" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="117"/>
-      <c r="D23" s="130" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="131"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="132"/>
-    </row>
-    <row r="24" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B24" s="117" t="s">
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
+      <c r="G27" s="127"/>
+      <c r="H27" s="127"/>
+      <c r="I27" s="127"/>
+      <c r="J27" s="127"/>
+      <c r="K27" s="127"/>
+      <c r="L27" s="127"/>
+    </row>
+    <row r="28" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B28" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="133" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="133"/>
-    </row>
-    <row r="25" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B25" s="117" t="s">
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="123"/>
+      <c r="I28" s="123"/>
+      <c r="J28" s="123"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="123"/>
+    </row>
+    <row r="29" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B29" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="117"/>
-      <c r="D25" s="133" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="133"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="133"/>
-      <c r="H25" s="133"/>
-      <c r="I25" s="133"/>
-      <c r="J25" s="133"/>
-      <c r="K25" s="133"/>
-      <c r="L25" s="133"/>
-    </row>
-    <row r="26" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B26" s="126" t="s">
+      <c r="C29" s="128"/>
+      <c r="D29" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
-      <c r="L26" s="126"/>
-    </row>
-    <row r="27" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B27" s="127" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="128"/>
-      <c r="D27" s="129" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="129"/>
-      <c r="F27" s="129"/>
-      <c r="G27" s="129"/>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-    </row>
-    <row r="28" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B28" s="125" t="s">
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="135"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="135"/>
+      <c r="J29" s="135"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="136"/>
+    </row>
+    <row r="30" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B30" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="125"/>
-    </row>
-    <row r="29" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B29" s="117" t="s">
+      <c r="C30" s="128"/>
+      <c r="D30" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="117"/>
-      <c r="D29" s="122" t="s">
+      <c r="E30" s="133"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="133"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="133"/>
+      <c r="J30" s="133"/>
+      <c r="K30" s="133"/>
+      <c r="L30" s="133"/>
+    </row>
+    <row r="31" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B31" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="123"/>
-      <c r="H29" s="123"/>
-      <c r="I29" s="123"/>
-      <c r="J29" s="123"/>
-      <c r="K29" s="123"/>
-      <c r="L29" s="124"/>
-    </row>
-    <row r="30" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B30" s="117" t="s">
+      <c r="C31" s="128"/>
+      <c r="D31" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="117"/>
-      <c r="D30" s="118" t="s">
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="133"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="133"/>
+      <c r="K31" s="133"/>
+      <c r="L31" s="133"/>
+    </row>
+    <row r="32" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B32" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-    </row>
-    <row r="31" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B31" s="117" t="s">
+      <c r="C32" s="128"/>
+      <c r="D32" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="117"/>
-      <c r="D31" s="118" t="s">
+      <c r="E32" s="133"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="133"/>
+      <c r="H32" s="133"/>
+      <c r="I32" s="133"/>
+      <c r="J32" s="133"/>
+      <c r="K32" s="133"/>
+      <c r="L32" s="133"/>
+    </row>
+    <row r="33" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B33" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="118"/>
-      <c r="K31" s="118"/>
-      <c r="L31" s="118"/>
-    </row>
-    <row r="32" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B32" s="117" t="s">
+      <c r="C33" s="128"/>
+      <c r="D33" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="117"/>
-      <c r="D32" s="118" t="s">
+      <c r="E33" s="133"/>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="133"/>
+      <c r="J33" s="133"/>
+      <c r="K33" s="133"/>
+      <c r="L33" s="133"/>
+    </row>
+    <row r="34" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B34" s="128" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="118"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="118"/>
-      <c r="H32" s="118"/>
-      <c r="I32" s="118"/>
-      <c r="J32" s="118"/>
-      <c r="K32" s="118"/>
-      <c r="L32" s="118"/>
-    </row>
-    <row r="33" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B33" s="117" t="s">
+      <c r="C34" s="128"/>
+      <c r="D34" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="117"/>
-      <c r="D33" s="118" t="s">
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="133"/>
+      <c r="H34" s="133"/>
+      <c r="I34" s="133"/>
+      <c r="J34" s="133"/>
+      <c r="K34" s="133"/>
+      <c r="L34" s="133"/>
+    </row>
+    <row r="35" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B35" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="118"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="118"/>
-    </row>
-    <row r="34" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B34" s="117" t="s">
+      <c r="C35" s="128"/>
+      <c r="D35" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="118" t="s">
+      <c r="E35" s="133"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="133"/>
+      <c r="H35" s="133"/>
+      <c r="I35" s="133"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="133"/>
+      <c r="L35" s="133"/>
+    </row>
+    <row r="36" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B36" s="144" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="118"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="118"/>
-      <c r="K34" s="118"/>
-      <c r="L34" s="118"/>
-    </row>
-    <row r="35" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B35" s="117" t="s">
+      <c r="C36" s="145"/>
+      <c r="D36" s="145"/>
+      <c r="E36" s="145"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="145"/>
+      <c r="I36" s="145"/>
+      <c r="J36" s="145"/>
+      <c r="K36" s="145"/>
+      <c r="L36" s="146"/>
+    </row>
+    <row r="37" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B37" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="118" t="s">
+      <c r="C37" s="128"/>
+      <c r="D37" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="118"/>
-      <c r="L35" s="118"/>
-    </row>
-    <row r="36" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B36" s="119" t="s">
+      <c r="E37" s="133"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="133"/>
+      <c r="H37" s="133"/>
+      <c r="I37" s="133"/>
+      <c r="J37" s="133"/>
+      <c r="K37" s="133"/>
+      <c r="L37" s="133"/>
+    </row>
+    <row r="38" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B38" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="120"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="120"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="121"/>
-    </row>
-    <row r="37" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B37" s="117" t="s">
+      <c r="C38" s="128"/>
+      <c r="D38" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="117"/>
-      <c r="D37" s="118" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="118"/>
-      <c r="L37" s="118"/>
-    </row>
-    <row r="38" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B38" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="117"/>
-      <c r="D38" s="118" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="118"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="118"/>
-      <c r="L38" s="118"/>
+      <c r="E38" s="133"/>
+      <c r="F38" s="133"/>
+      <c r="G38" s="133"/>
+      <c r="H38" s="133"/>
+      <c r="I38" s="133"/>
+      <c r="J38" s="133"/>
+      <c r="K38" s="133"/>
+      <c r="L38" s="133"/>
     </row>
     <row r="39" spans="2:12" ht="24.95" customHeight="1">
-      <c r="B39" s="108" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="108"/>
-      <c r="D39" s="109" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="109"/>
-      <c r="F39" s="109"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="109"/>
-      <c r="J39" s="109"/>
-      <c r="K39" s="109"/>
-      <c r="L39" s="109"/>
+      <c r="B39" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="137"/>
+      <c r="D39" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="138"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="138"/>
+      <c r="H39" s="138"/>
+      <c r="I39" s="138"/>
+      <c r="J39" s="138"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="138"/>
     </row>
     <row r="40" spans="2:12">
       <c r="B40" s="4"/>
@@ -3433,40 +3442,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:L10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:L12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:L14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:L16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:L18"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:L22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:L23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:L24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:L27"/>
-    <mergeCell ref="D33:L33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:L34"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:L29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:L30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:L31"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:L39"/>
     <mergeCell ref="B1:L5"/>
@@ -3483,6 +3458,40 @@
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:L32"/>
     <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:L33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:L34"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:L29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:L30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:L31"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:L22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:L23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:L24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:L27"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:L14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:L10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3494,18 +3503,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J10" sqref="A6:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.5703125" style="77" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="147" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="148"/>
       <c r="C1" s="148"/>
@@ -3627,7 +3637,7 @@
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1">
       <c r="A6" s="171" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B6" s="172"/>
       <c r="C6" s="172"/>
@@ -3655,11 +3665,11 @@
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="177" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="178"/>
       <c r="C8" s="179" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="180"/>
       <c r="E8" s="180"/>
@@ -3672,11 +3682,11 @@
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1">
       <c r="A9" s="177" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="178"/>
       <c r="C9" s="179" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="180"/>
       <c r="E9" s="180"/>
@@ -3708,7 +3718,7 @@
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="156" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="157"/>
       <c r="H12" s="157"/>
@@ -3731,1206 +3741,1206 @@
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="159" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G13" s="160"/>
       <c r="H13" s="161"/>
       <c r="I13" s="162" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J13" s="163"/>
       <c r="K13" s="164"/>
       <c r="L13" s="165" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="M13" s="166"/>
       <c r="N13" s="166"/>
       <c r="O13" s="166"/>
       <c r="P13" s="167"/>
       <c r="Q13" s="168" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="R13" s="169"/>
       <c r="S13" s="170"/>
     </row>
     <row r="14" spans="1:22" ht="38.25">
       <c r="A14" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="O14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="P14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="18" t="s">
+      <c r="R14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="S14" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="45" customHeight="1">
+      <c r="A15" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="M14" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="19" t="s">
+      <c r="B15" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="O14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="18" t="s">
+      <c r="D15" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="S14" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="38.25">
-      <c r="A15" s="78" t="s">
+      <c r="E15" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="23" t="s">
+      <c r="F15" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="85" t="s">
+      <c r="G15" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I15" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J15" s="24">
         <v>5</v>
       </c>
       <c r="K15" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="R15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="S15" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="45" customHeight="1">
+      <c r="A16" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="L15" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="M15" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N15" s="28" t="s">
+      <c r="B16" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="O15" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="P15" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q15" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="R15" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="S15" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="38.25">
-      <c r="A16" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>70</v>
-      </c>
       <c r="C16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="85" t="s">
+      <c r="G16" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I16" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J16" s="24">
         <v>5</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M16" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O16" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P16" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q16" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="S16" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="45" customHeight="1">
+      <c r="A17" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="B17" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="R16" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="S16" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="38.25">
-      <c r="A17" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="71" t="s">
-        <v>72</v>
-      </c>
       <c r="C17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="85" t="s">
+      <c r="G17" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I17" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J17" s="24">
         <v>5</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M17" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N17" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O17" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P17" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q17" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S17" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="51">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="45" customHeight="1">
       <c r="A18" s="79" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="85" t="s">
+      <c r="G18" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I18" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J18" s="24">
         <v>5</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M18" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O18" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P18" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S18" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="45" customHeight="1">
       <c r="A19" s="79" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="85" t="s">
+      <c r="G19" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I19" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J19" s="24">
         <v>5</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O19" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S19" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="45" customHeight="1">
       <c r="A20" s="79" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="85" t="s">
+      <c r="G20" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I20" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J20" s="24">
         <v>5</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M20" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M20" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O20" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S20" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="45" customHeight="1">
       <c r="A21" s="79" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="85" t="s">
+      <c r="G21" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I21" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J21" s="24">
         <v>5</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L21" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N21" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q21" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S21" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="45" customHeight="1">
       <c r="A22" s="79" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B22" s="72" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C22" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="85" t="s">
+      <c r="G22" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I22" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J22" s="24">
         <v>5</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M22" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N22" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q22" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S22" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="45" customHeight="1">
       <c r="A23" s="78" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C23" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="85" t="s">
+      <c r="G23" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I23" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J23" s="24">
         <v>5</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L23" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M23" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N23" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O23" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q23" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R23" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S23" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="45" customHeight="1">
       <c r="A24" s="79" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" s="71" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="85" t="s">
+      <c r="G24" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I24" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J24" s="24">
         <v>5</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="M24" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N24" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O24" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P24" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q24" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S24" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="45" customHeight="1">
       <c r="A25" s="79" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B25" s="71" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="85" t="s">
+      <c r="G25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I25" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J25" s="24">
         <v>5</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="M25" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N25" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O25" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q25" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S25" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="51">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="45" customHeight="1">
       <c r="A26" s="79" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" s="71" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="85" t="s">
+      <c r="G26" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I26" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J26" s="24">
         <v>5</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="M26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M26" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N26" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O26" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q26" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S26" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="45" customHeight="1">
       <c r="A27" s="78" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="85" t="s">
+      <c r="G27" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I27" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J27" s="24">
         <v>5</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L27" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="M27" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M27" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N27" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O27" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P27" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q27" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R27" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S27" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="45" customHeight="1">
       <c r="A28" s="79" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B28" s="72" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C28" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="85" t="s">
+      <c r="G28" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I28" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J28" s="24">
         <v>5</v>
       </c>
       <c r="K28" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L28" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="M28" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M28" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N28" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O28" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P28" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q28" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R28" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S28" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="45" customHeight="1">
       <c r="A29" s="78" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C29" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="85" t="s">
+      <c r="G29" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I29" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J29" s="24">
         <v>5</v>
       </c>
       <c r="K29" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L29" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M29" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N29" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O29" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P29" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q29" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R29" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S29" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="45" customHeight="1">
       <c r="A30" s="79" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B30" s="71" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C30" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="85" t="s">
+      <c r="G30" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I30" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J30" s="24">
         <v>5</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L30" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="M30" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M30" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N30" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O30" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P30" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q30" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R30" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S30" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="45" customHeight="1">
       <c r="A31" s="79" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B31" s="71" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="85" t="s">
+      <c r="G31" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I31" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J31" s="24">
         <v>5</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L31" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="M31" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M31" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N31" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O31" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P31" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q31" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R31" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S31" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="38.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="45" customHeight="1">
       <c r="A32" s="79" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B32" s="74" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="85" t="s">
+      <c r="G32" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="I32" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J32" s="24">
         <v>5</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L32" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L32" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="M32" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M32" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N32" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="O32" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P32" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q32" s="27" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R32" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S32" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="39" thickBot="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="45" customHeight="1" thickBot="1">
       <c r="A33" s="80" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C33" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="30" t="s">
+      <c r="G33" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>64</v>
-      </c>
       <c r="I33" s="33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J33" s="32">
         <v>5</v>
       </c>
       <c r="K33" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="L33" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L33" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="M33" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="M33" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="N33" s="34" t="s">
-        <v>66</v>
-      </c>
       <c r="O33" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P33" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q33" s="33" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="R33" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S33" s="30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -4958,7 +4968,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4986,21 +4997,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="15.75" thickBot="1">
-      <c r="A1" s="198" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="201" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
-      <c r="K1" s="203"/>
+      <c r="A1" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="183"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="187"/>
     </row>
     <row r="2" spans="1:47" ht="15.75" thickBot="1">
       <c r="A2" s="14"/>
@@ -5019,50 +5030,50 @@
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="185" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="186"/>
-      <c r="M3" s="186"/>
-      <c r="N3" s="186"/>
-      <c r="O3" s="186"/>
-      <c r="P3" s="186"/>
-      <c r="Q3" s="186"/>
-      <c r="R3" s="186"/>
-      <c r="S3" s="186"/>
-      <c r="T3" s="186"/>
-      <c r="U3" s="186"/>
-      <c r="V3" s="186"/>
-      <c r="W3" s="186"/>
-      <c r="X3" s="186"/>
-      <c r="Y3" s="186"/>
-      <c r="Z3" s="186"/>
-      <c r="AA3" s="186"/>
-      <c r="AB3" s="186"/>
-      <c r="AC3" s="186"/>
-      <c r="AD3" s="186"/>
-      <c r="AE3" s="186"/>
-      <c r="AF3" s="186"/>
-      <c r="AG3" s="186"/>
-      <c r="AH3" s="186"/>
-      <c r="AI3" s="186"/>
-      <c r="AJ3" s="186"/>
-      <c r="AK3" s="186"/>
-      <c r="AL3" s="186"/>
-      <c r="AM3" s="186"/>
-      <c r="AN3" s="186"/>
-      <c r="AO3" s="186"/>
-      <c r="AP3" s="186"/>
-      <c r="AQ3" s="186"/>
-      <c r="AR3" s="186"/>
-      <c r="AS3" s="186"/>
-      <c r="AT3" s="186"/>
-      <c r="AU3" s="187"/>
+      <c r="F3" s="191" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
+      <c r="T3" s="192"/>
+      <c r="U3" s="192"/>
+      <c r="V3" s="192"/>
+      <c r="W3" s="192"/>
+      <c r="X3" s="192"/>
+      <c r="Y3" s="192"/>
+      <c r="Z3" s="192"/>
+      <c r="AA3" s="192"/>
+      <c r="AB3" s="192"/>
+      <c r="AC3" s="192"/>
+      <c r="AD3" s="192"/>
+      <c r="AE3" s="192"/>
+      <c r="AF3" s="192"/>
+      <c r="AG3" s="192"/>
+      <c r="AH3" s="192"/>
+      <c r="AI3" s="192"/>
+      <c r="AJ3" s="192"/>
+      <c r="AK3" s="192"/>
+      <c r="AL3" s="192"/>
+      <c r="AM3" s="192"/>
+      <c r="AN3" s="192"/>
+      <c r="AO3" s="192"/>
+      <c r="AP3" s="192"/>
+      <c r="AQ3" s="192"/>
+      <c r="AR3" s="192"/>
+      <c r="AS3" s="192"/>
+      <c r="AT3" s="192"/>
+      <c r="AU3" s="193"/>
     </row>
     <row r="4" spans="1:47" ht="18.75" thickBot="1">
       <c r="A4" s="15"/>
@@ -5070,54 +5081,54 @@
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
-      <c r="F4" s="188" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="189"/>
-      <c r="H4" s="189"/>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
-      <c r="K4" s="189"/>
-      <c r="L4" s="189"/>
-      <c r="M4" s="189"/>
-      <c r="N4" s="190"/>
-      <c r="O4" s="191" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="192"/>
-      <c r="Q4" s="192"/>
-      <c r="R4" s="192"/>
-      <c r="S4" s="192"/>
-      <c r="T4" s="192"/>
-      <c r="U4" s="192"/>
-      <c r="V4" s="192"/>
-      <c r="W4" s="192"/>
-      <c r="X4" s="192"/>
-      <c r="Y4" s="192"/>
-      <c r="Z4" s="192"/>
-      <c r="AA4" s="192"/>
-      <c r="AB4" s="192"/>
-      <c r="AC4" s="192"/>
-      <c r="AD4" s="192"/>
-      <c r="AE4" s="192"/>
-      <c r="AF4" s="192"/>
-      <c r="AG4" s="192"/>
-      <c r="AH4" s="192"/>
-      <c r="AI4" s="192"/>
-      <c r="AJ4" s="192"/>
-      <c r="AK4" s="192"/>
-      <c r="AL4" s="193"/>
-      <c r="AM4" s="191" t="s">
-        <v>106</v>
-      </c>
-      <c r="AN4" s="192"/>
-      <c r="AO4" s="192"/>
-      <c r="AP4" s="192"/>
-      <c r="AQ4" s="192"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
-      <c r="AU4" s="193"/>
+      <c r="F4" s="194" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="195"/>
+      <c r="H4" s="195"/>
+      <c r="I4" s="195"/>
+      <c r="J4" s="195"/>
+      <c r="K4" s="195"/>
+      <c r="L4" s="195"/>
+      <c r="M4" s="195"/>
+      <c r="N4" s="196"/>
+      <c r="O4" s="197" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" s="198"/>
+      <c r="Q4" s="198"/>
+      <c r="R4" s="198"/>
+      <c r="S4" s="198"/>
+      <c r="T4" s="198"/>
+      <c r="U4" s="198"/>
+      <c r="V4" s="198"/>
+      <c r="W4" s="198"/>
+      <c r="X4" s="198"/>
+      <c r="Y4" s="198"/>
+      <c r="Z4" s="198"/>
+      <c r="AA4" s="198"/>
+      <c r="AB4" s="198"/>
+      <c r="AC4" s="198"/>
+      <c r="AD4" s="198"/>
+      <c r="AE4" s="198"/>
+      <c r="AF4" s="198"/>
+      <c r="AG4" s="198"/>
+      <c r="AH4" s="198"/>
+      <c r="AI4" s="198"/>
+      <c r="AJ4" s="198"/>
+      <c r="AK4" s="198"/>
+      <c r="AL4" s="199"/>
+      <c r="AM4" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN4" s="198"/>
+      <c r="AO4" s="198"/>
+      <c r="AP4" s="198"/>
+      <c r="AQ4" s="198"/>
+      <c r="AR4" s="198"/>
+      <c r="AS4" s="198"/>
+      <c r="AT4" s="198"/>
+      <c r="AU4" s="199"/>
     </row>
     <row r="5" spans="1:47" s="57" customFormat="1" ht="36.75" customHeight="1" thickBot="1">
       <c r="A5" s="67"/>
@@ -5126,22 +5137,22 @@
       <c r="D5" s="67"/>
       <c r="E5" s="67"/>
       <c r="F5" s="159" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G5" s="160"/>
       <c r="H5" s="161"/>
       <c r="I5" s="162" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J5" s="163"/>
       <c r="K5" s="164"/>
-      <c r="L5" s="194" t="s">
-        <v>108</v>
-      </c>
-      <c r="M5" s="194"/>
-      <c r="N5" s="194"/>
+      <c r="L5" s="200" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
       <c r="O5" s="159" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P5" s="160"/>
       <c r="Q5" s="160"/>
@@ -5149,36 +5160,36 @@
       <c r="S5" s="160"/>
       <c r="T5" s="161"/>
       <c r="U5" s="162" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="V5" s="163"/>
       <c r="W5" s="163"/>
       <c r="X5" s="163"/>
       <c r="Y5" s="163"/>
       <c r="Z5" s="164"/>
-      <c r="AA5" s="195" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB5" s="196"/>
-      <c r="AC5" s="196"/>
-      <c r="AD5" s="196"/>
-      <c r="AE5" s="196"/>
-      <c r="AF5" s="197"/>
-      <c r="AG5" s="182" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH5" s="183"/>
-      <c r="AI5" s="183"/>
-      <c r="AJ5" s="183"/>
-      <c r="AK5" s="183"/>
-      <c r="AL5" s="184"/>
+      <c r="AA5" s="201" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB5" s="202"/>
+      <c r="AC5" s="202"/>
+      <c r="AD5" s="202"/>
+      <c r="AE5" s="202"/>
+      <c r="AF5" s="203"/>
+      <c r="AG5" s="188" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH5" s="189"/>
+      <c r="AI5" s="189"/>
+      <c r="AJ5" s="189"/>
+      <c r="AK5" s="189"/>
+      <c r="AL5" s="190"/>
       <c r="AM5" s="159" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AN5" s="160"/>
       <c r="AO5" s="161"/>
       <c r="AP5" s="162" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AQ5" s="163"/>
       <c r="AR5" s="163"/>
@@ -5188,153 +5199,153 @@
     </row>
     <row r="6" spans="1:47" s="66" customFormat="1" ht="48" customHeight="1">
       <c r="A6" s="58" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="S6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="61" t="s">
+      <c r="V6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="61" t="s">
+      <c r="Y6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA6" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="M6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="P6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q6" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" s="63" t="s">
+      <c r="AE6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG6" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="S6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="T6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="61" t="s">
+      <c r="AH6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI6" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ6" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="V6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="W6" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="X6" s="63" t="s">
+      <c r="AK6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM6" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="Y6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA6" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC6" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD6" s="63" t="s">
+      <c r="AN6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP6" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="AE6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG6" s="64" t="s">
+      <c r="AQ6" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR6" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS6" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="AH6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI6" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ6" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="AK6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM6" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="AN6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO6" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP6" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR6" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS6" s="64" t="s">
-        <v>126</v>
-      </c>
       <c r="AT6" s="59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AU6" s="60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:47" ht="80.25" customHeight="1">
       <c r="A7" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="39"/>
@@ -5384,10 +5395,10 @@
     </row>
     <row r="8" spans="1:47" ht="88.5" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
@@ -5437,10 +5448,10 @@
     </row>
     <row r="9" spans="1:47" ht="45">
       <c r="A9" s="36" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>

</xml_diff>